<commit_message>
sumeyra API last commit
</commit_message>
<xml_diff>
--- a/src/test/resources/ids.xlsx
+++ b/src/test/resources/ids.xlsx
@@ -457,13 +457,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="n" s="0">
-        <v>120.0</v>
+        <v>130.0</v>
       </c>
       <c r="B2" s="0">
         <v>20</v>
       </c>
-      <c r="C2" s="0">
-        <v>30</v>
+      <c r="C2" s="0" t="n">
+        <v>234.0</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>76.0</v>

</xml_diff>

<commit_message>
Yigit Framework extended to include DATABASE features.
</commit_message>
<xml_diff>
--- a/src/test/resources/ids.xlsx
+++ b/src/test/resources/ids.xlsx
@@ -457,7 +457,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="n" s="0">
-        <v>139.0</v>
+        <v>144.0</v>
       </c>
       <c r="B2" s="0">
         <v>20</v>
@@ -466,7 +466,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>107.0</v>
+        <v>109.0</v>
       </c>
       <c r="E2" s="0">
         <v>50</v>

</xml_diff>